<commit_message>
Added Data to Investigation with ARCitect
</commit_message>
<xml_diff>
--- a/isa.investigation.xlsx
+++ b/isa.investigation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -34,15 +34,22 @@
     <t>Investigation Identifier</t>
   </si>
   <si>
-    <t>testarc</t>
+    <t>M4.4_UC6_ARC</t>
   </si>
   <si>
     <t>Investigation Title</t>
   </si>
   <si>
+    <t>ARC for UC6</t>
+  </si>
+  <si>
     <t>Investigation Description</t>
   </si>
   <si>
+    <t xml:space="preserve">In this repository, we will create an annotated research context ARC with assays, studies, workflows and runs of these workflows for Use Case 6 of FAIRagro. Use Case 6 deals with ETL functions for semiautomated data integration into crop simulation modelling.
+The ARC contians a modularised CWL workflow that can be executed locally with cwltool. To facilitate writing CWL, a minimal templating system that helps to generate CWL will be used or developed. Once the finalised ARC has undergone a test to verify that the workflow is running as intended, it will also be made accessible via the PLANTdataHUB. The ARC will serve as a test case for the further development of a Scientific Workflow Infrastructure (SciWIn).</t>
+  </si>
+  <si>
     <t>Investigation Submission Date</t>
   </si>
   <si>
@@ -79,15 +86,45 @@
     <t>Investigation Person Last Name</t>
   </si>
   <si>
+    <t>Krumsieck</t>
+  </si>
+  <si>
+    <t>Leidel</t>
+  </si>
+  <si>
+    <t>König</t>
+  </si>
+  <si>
+    <t>von Waldow</t>
+  </si>
+  <si>
     <t>Investigation Person First Name</t>
   </si>
   <si>
+    <t>Jens</t>
+  </si>
+  <si>
+    <t>Antonia</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Harald</t>
+  </si>
+  <si>
     <t>Investigation Person Mid Initials</t>
   </si>
   <si>
     <t>Investigation Person Email</t>
   </si>
   <si>
+    <t>jens.krumsieck@thuenen.de</t>
+  </si>
+  <si>
+    <t>harald.vonwaldow@thuenen.de</t>
+  </si>
+  <si>
     <t>Investigation Person Phone</t>
   </si>
   <si>
@@ -100,13 +137,43 @@
     <t>Investigation Person Affiliation</t>
   </si>
   <si>
+    <t>Johann Heinrich von Thünen-Institut, Zentrum für Informationsmanagement;Technische Universität Braunschweig, Institut für Anorganische und Analytische Chemie</t>
+  </si>
+  <si>
+    <t>Leibniz Institute of Plant Genetics and Crop Plant Research (IPK), Department of Breeding Research</t>
+  </si>
+  <si>
+    <t>Johann Heinrich von Thünen-Institut, Centre for Information Management;Eawag, IT Services</t>
+  </si>
+  <si>
     <t>Investigation Person Roles</t>
   </si>
   <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
     <t>Investigation Person Roles Term Accession Number</t>
   </si>
   <si>
+    <t>NCIT:C19924</t>
+  </si>
+  <si>
     <t>Investigation Person Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>Comment[ORCID]</t>
+  </si>
+  <si>
+    <t>0000-0001-6242-5846</t>
+  </si>
+  <si>
+    <t>0000-0002-8948-6793</t>
+  </si>
+  <si>
+    <t>0000-0003-4800-2833</t>
   </si>
 </sst>
 </file>
@@ -458,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:E32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -499,124 +566,195 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>